<commit_message>
Results as XLSX file
</commit_message>
<xml_diff>
--- a/Data/somResults/wade/2020-11-18/Results_wade_4_cl.xlsx
+++ b/Data/somResults/wade/2020-11-18/Results_wade_4_cl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinkincaid/ownCloud/BREE/Watershed Data/1_Projects/FluxRegimes/Data/somResults/wade/2020-11-18/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88E645D4-965F-FF4E-8E35-C04E4E58F7F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EB19DBCB-3450-604B-9F70-D87FD5E338A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="24">
   <si>
     <t>Run</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>noPCA</t>
+  </si>
+  <si>
+    <t>target nodes: 48</t>
+  </si>
+  <si>
+    <t>target col/row ratio: 1.3</t>
   </si>
 </sst>
 </file>
@@ -228,7 +234,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,6 +412,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -569,8 +581,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -627,6 +640,1092 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Results_wade_4_cl!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>QE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Results_wade_4_cl!$O$2:$O$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.118973</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13566400000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19780500000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15814900000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13056100000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.14791499999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.137517</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20116100000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.15381500000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.19908600000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.17085</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.13392899999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.17452200000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.163518</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1FA4-044F-8FC1-074EA16F6FF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1332125583"/>
+        <c:axId val="1279124143"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Results_wade_4_cl!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>npF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Results_wade_4_cl!$P$2:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>44.439588000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.270493000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.857452000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.646991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.329815000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42.890416999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41.597572</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40.803859000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39.443378000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36.077903999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36.047210999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35.358454999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>31.989055</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26.932995999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1FA4-044F-8FC1-074EA16F6FF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1279135487"/>
+        <c:axId val="1279133839"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1332125583"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1279124143"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1279124143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1332125583"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1279133839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1279135487"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1279135487"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1279133839"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>692150</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E21A977D-2891-1D49-97D5-501AB829A8A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -926,9 +2025,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -989,135 +2090,135 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="1">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="1">
+        <v>54</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="E2" s="1">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>1000</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>0.05</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="1">
         <v>0.01</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>4</v>
       </c>
-      <c r="M2">
-        <v>1.4</v>
-      </c>
-      <c r="N2">
-        <v>0.201160667762077</v>
-      </c>
-      <c r="O2">
-        <v>0.20116100000000001</v>
-      </c>
-      <c r="P2">
-        <v>40.803859000000003</v>
-      </c>
-      <c r="Q2">
+      <c r="M2" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0.11897348684291</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0.118973</v>
+      </c>
+      <c r="P2" s="1">
+        <v>44.439588000000001</v>
+      </c>
+      <c r="Q2" s="1">
         <v>0.01</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="1">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="1">
+        <v>56</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
+      <c r="E3" s="1">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1">
         <v>8</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>1000</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>0.05</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="1">
         <v>0.01</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1">
         <v>4</v>
       </c>
-      <c r="M3">
-        <v>1.6</v>
-      </c>
-      <c r="N3">
-        <v>0.16351833802816301</v>
-      </c>
-      <c r="O3">
-        <v>0.163518</v>
-      </c>
-      <c r="P3">
-        <v>26.932995999999999</v>
-      </c>
-      <c r="Q3">
+      <c r="M3" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.13566393541079499</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.13566400000000001</v>
+      </c>
+      <c r="P3" s="1">
+        <v>44.270493000000002</v>
+      </c>
+      <c r="Q3" s="1">
         <v>0.01</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
         <v>20</v>
@@ -1138,16 +2239,16 @@
         <v>4</v>
       </c>
       <c r="M4">
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
       <c r="N4">
-        <v>0.15381514177835501</v>
+        <v>0.197805196643386</v>
       </c>
       <c r="O4">
-        <v>0.15381500000000001</v>
+        <v>0.19780500000000001</v>
       </c>
       <c r="P4">
-        <v>39.443378000000003</v>
+        <v>43.857452000000002</v>
       </c>
       <c r="Q4">
         <v>0.01</v>
@@ -1158,22 +2259,22 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F5">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
@@ -1194,16 +2295,16 @@
         <v>4</v>
       </c>
       <c r="M5">
-        <v>2</v>
+        <v>0.8</v>
       </c>
       <c r="N5">
-        <v>0.133929429571544</v>
+        <v>0.15814869426327199</v>
       </c>
       <c r="O5">
-        <v>0.13392899999999999</v>
+        <v>0.15814900000000001</v>
       </c>
       <c r="P5">
-        <v>35.358454999999999</v>
+        <v>43.646991</v>
       </c>
       <c r="Q5">
         <v>0.01</v>
@@ -1213,76 +2314,76 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>55</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>5</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>11</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <v>1000</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>0.05</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="1">
         <v>0.01</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="1">
         <v>4</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="1">
         <v>0.130560711367296</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="1">
         <v>0.13056100000000001</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="1">
         <v>43.329815000000004</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="1">
         <v>0.01</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
       <c r="C7">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F7">
         <v>7</v>
@@ -1306,16 +2407,16 @@
         <v>4</v>
       </c>
       <c r="M7">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="N7">
-        <v>0.197805196643386</v>
+        <v>0.14791452419828699</v>
       </c>
       <c r="O7">
-        <v>0.19780500000000001</v>
+        <v>0.14791499999999999</v>
       </c>
       <c r="P7">
-        <v>43.857452000000002</v>
+        <v>42.890416999999999</v>
       </c>
       <c r="Q7">
         <v>0.01</v>
@@ -1382,22 +2483,22 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
       </c>
       <c r="E9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G9" t="s">
         <v>20</v>
@@ -1418,16 +2519,16 @@
         <v>4</v>
       </c>
       <c r="M9">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="N9">
-        <v>0.11897348684291</v>
+        <v>0.201160667762077</v>
       </c>
       <c r="O9">
-        <v>0.118973</v>
+        <v>0.20116100000000001</v>
       </c>
       <c r="P9">
-        <v>44.439588000000001</v>
+        <v>40.803859000000003</v>
       </c>
       <c r="Q9">
         <v>0.01</v>
@@ -1438,22 +2539,22 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="C10">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="E10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F10">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G10" t="s">
         <v>20</v>
@@ -1474,16 +2575,16 @@
         <v>4</v>
       </c>
       <c r="M10">
-        <v>0.9</v>
+        <v>1.8</v>
       </c>
       <c r="N10">
-        <v>0.19908614008276401</v>
+        <v>0.15381514177835501</v>
       </c>
       <c r="O10">
-        <v>0.19908600000000001</v>
+        <v>0.15381500000000001</v>
       </c>
       <c r="P10">
-        <v>36.077903999999997</v>
+        <v>39.443378000000003</v>
       </c>
       <c r="Q10">
         <v>0.01</v>
@@ -1494,13 +2595,13 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
       <c r="C11">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
@@ -1509,7 +2610,7 @@
         <v>7</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11" t="s">
         <v>20</v>
@@ -1530,16 +2631,16 @@
         <v>4</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="N11">
-        <v>0.14791452419828699</v>
+        <v>0.19908614008276401</v>
       </c>
       <c r="O11">
-        <v>0.14791499999999999</v>
+        <v>0.19908600000000001</v>
       </c>
       <c r="P11">
-        <v>42.890416999999999</v>
+        <v>36.077903999999997</v>
       </c>
       <c r="Q11">
         <v>0.01</v>
@@ -1550,7 +2651,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -1562,10 +2663,10 @@
         <v>19</v>
       </c>
       <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12">
         <v>7</v>
-      </c>
-      <c r="F12">
-        <v>8</v>
       </c>
       <c r="G12" t="s">
         <v>20</v>
@@ -1586,16 +2687,16 @@
         <v>4</v>
       </c>
       <c r="M12">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="N12">
-        <v>0.13566393541079499</v>
+        <v>0.17084959716324799</v>
       </c>
       <c r="O12">
-        <v>0.13566400000000001</v>
+        <v>0.17085</v>
       </c>
       <c r="P12">
-        <v>44.270493000000002</v>
+        <v>36.047210999999997</v>
       </c>
       <c r="Q12">
         <v>0.01</v>
@@ -1606,22 +2707,22 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
       </c>
       <c r="C13">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
         <v>19</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G13" t="s">
         <v>20</v>
@@ -1642,16 +2743,16 @@
         <v>4</v>
       </c>
       <c r="M13">
-        <v>0.6</v>
+        <v>2</v>
       </c>
       <c r="N13">
-        <v>0.174521922792721</v>
+        <v>0.133929429571544</v>
       </c>
       <c r="O13">
-        <v>0.17452200000000001</v>
+        <v>0.13392899999999999</v>
       </c>
       <c r="P13">
-        <v>31.989055</v>
+        <v>35.358454999999999</v>
       </c>
       <c r="Q13">
         <v>0.01</v>
@@ -1662,13 +2763,13 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
       <c r="C14">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
@@ -1677,7 +2778,7 @@
         <v>8</v>
       </c>
       <c r="F14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G14" t="s">
         <v>20</v>
@@ -1698,16 +2799,16 @@
         <v>4</v>
       </c>
       <c r="M14">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="N14">
-        <v>0.15814869426327199</v>
+        <v>0.174521922792721</v>
       </c>
       <c r="O14">
-        <v>0.15814900000000001</v>
+        <v>0.17452200000000001</v>
       </c>
       <c r="P14">
-        <v>43.646991</v>
+        <v>31.989055</v>
       </c>
       <c r="Q14">
         <v>0.01</v>
@@ -1718,22 +2819,22 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
         <v>19</v>
       </c>
       <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
         <v>8</v>
-      </c>
-      <c r="F15">
-        <v>7</v>
       </c>
       <c r="G15" t="s">
         <v>20</v>
@@ -1754,16 +2855,16 @@
         <v>4</v>
       </c>
       <c r="M15">
-        <v>0.9</v>
+        <v>1.6</v>
       </c>
       <c r="N15">
-        <v>0.17084959716324799</v>
+        <v>0.16351833802816301</v>
       </c>
       <c r="O15">
-        <v>0.17085</v>
+        <v>0.163518</v>
       </c>
       <c r="P15">
-        <v>36.047210999999997</v>
+        <v>26.932995999999999</v>
       </c>
       <c r="Q15">
         <v>0.01</v>
@@ -1772,7 +2873,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1"/>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R15">
+    <sortCondition descending="1" ref="P2:P15"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>